<commit_message>
add a new file named GSB_test.py
Signed-off-by: zuosong <zu.so@163.com>
</commit_message>
<xml_diff>
--- a/Gongsibao/file.xlsx
+++ b/Gongsibao/file.xlsx
@@ -4,14 +4,13 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17610" windowHeight="11730" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17610" windowHeight="11730" activeTab="3"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet2" sheetId="4" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="5" r:id="rId2"/>
-    <sheet name="官网" sheetId="1" r:id="rId3"/>
-    <sheet name="推广" sheetId="2" r:id="rId4"/>
-    <sheet name="商品页" sheetId="3" r:id="rId5"/>
+    <sheet name="Sheet1" sheetId="5" r:id="rId1"/>
+    <sheet name="官网" sheetId="1" r:id="rId2"/>
+    <sheet name="推广" sheetId="2" r:id="rId3"/>
+    <sheet name="商品页" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
@@ -824,7 +823,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -909,29 +908,71 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -942,18 +983,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -975,44 +1007,8 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1311,425 +1307,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F20"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K20" sqref="K20"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
-  <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1">
-        <v>1</v>
-      </c>
-      <c r="B1" s="28">
-        <v>2</v>
-      </c>
-      <c r="C1" s="28">
-        <v>3</v>
-      </c>
-      <c r="D1" s="28">
-        <v>4</v>
-      </c>
-      <c r="E1" s="28">
-        <v>5</v>
-      </c>
-      <c r="F1" s="28">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
-      <c r="A2" s="28">
-        <v>2</v>
-      </c>
-      <c r="B2" s="28">
-        <v>3</v>
-      </c>
-      <c r="C2" s="28">
-        <v>4</v>
-      </c>
-      <c r="D2" s="28">
-        <v>5</v>
-      </c>
-      <c r="E2" s="28">
-        <v>6</v>
-      </c>
-      <c r="F2" s="28">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="A3" s="28">
-        <v>3</v>
-      </c>
-      <c r="B3" s="28">
-        <v>4</v>
-      </c>
-      <c r="C3" s="28">
-        <v>5</v>
-      </c>
-      <c r="D3" s="28">
-        <v>6</v>
-      </c>
-      <c r="E3" s="28">
-        <v>7</v>
-      </c>
-      <c r="F3" s="28">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4" s="28">
-        <v>4</v>
-      </c>
-      <c r="B4" s="28">
-        <v>5</v>
-      </c>
-      <c r="C4" s="28">
-        <v>6</v>
-      </c>
-      <c r="D4" s="28">
-        <v>7</v>
-      </c>
-      <c r="E4" s="28">
-        <v>8</v>
-      </c>
-      <c r="F4" s="28">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5" s="28">
-        <v>5</v>
-      </c>
-      <c r="B5" s="28">
-        <v>6</v>
-      </c>
-      <c r="C5" s="28">
-        <v>7</v>
-      </c>
-      <c r="D5" s="28">
-        <v>8</v>
-      </c>
-      <c r="E5" s="28">
-        <v>9</v>
-      </c>
-      <c r="F5" s="28">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="A6" s="28">
-        <v>6</v>
-      </c>
-      <c r="B6" s="28">
-        <v>7</v>
-      </c>
-      <c r="C6" s="28">
-        <v>8</v>
-      </c>
-      <c r="D6" s="28">
-        <v>9</v>
-      </c>
-      <c r="E6" s="28">
-        <v>10</v>
-      </c>
-      <c r="F6" s="28">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
-      <c r="A7" s="28">
-        <v>7</v>
-      </c>
-      <c r="B7" s="28">
-        <v>8</v>
-      </c>
-      <c r="C7" s="28">
-        <v>9</v>
-      </c>
-      <c r="D7" s="28">
-        <v>10</v>
-      </c>
-      <c r="E7" s="28">
-        <v>11</v>
-      </c>
-      <c r="F7" s="28">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="A8" s="28">
-        <v>8</v>
-      </c>
-      <c r="B8" s="28">
-        <v>9</v>
-      </c>
-      <c r="C8" s="28">
-        <v>10</v>
-      </c>
-      <c r="D8" s="28">
-        <v>11</v>
-      </c>
-      <c r="E8" s="28">
-        <v>12</v>
-      </c>
-      <c r="F8" s="28">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
-      <c r="A9" s="28">
-        <v>9</v>
-      </c>
-      <c r="B9" s="28">
-        <v>10</v>
-      </c>
-      <c r="C9" s="28">
-        <v>11</v>
-      </c>
-      <c r="D9" s="28">
-        <v>12</v>
-      </c>
-      <c r="E9" s="28">
-        <v>13</v>
-      </c>
-      <c r="F9" s="28">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
-      <c r="A10" s="28">
-        <v>10</v>
-      </c>
-      <c r="B10" s="28">
-        <v>11</v>
-      </c>
-      <c r="C10" s="28">
-        <v>12</v>
-      </c>
-      <c r="D10" s="28">
-        <v>13</v>
-      </c>
-      <c r="E10" s="28">
-        <v>14</v>
-      </c>
-      <c r="F10" s="28">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6">
-      <c r="A11" s="28">
-        <v>11</v>
-      </c>
-      <c r="B11" s="28">
-        <v>12</v>
-      </c>
-      <c r="C11" s="28">
-        <v>13</v>
-      </c>
-      <c r="D11" s="28">
-        <v>14</v>
-      </c>
-      <c r="E11" s="28">
-        <v>15</v>
-      </c>
-      <c r="F11" s="28">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6">
-      <c r="A12" s="28">
-        <v>12</v>
-      </c>
-      <c r="B12" s="28">
-        <v>13</v>
-      </c>
-      <c r="C12" s="28">
-        <v>14</v>
-      </c>
-      <c r="D12" s="28">
-        <v>15</v>
-      </c>
-      <c r="E12" s="28">
-        <v>16</v>
-      </c>
-      <c r="F12" s="28">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6">
-      <c r="A13" s="28">
-        <v>13</v>
-      </c>
-      <c r="B13" s="28">
-        <v>14</v>
-      </c>
-      <c r="C13" s="28">
-        <v>15</v>
-      </c>
-      <c r="D13" s="28">
-        <v>16</v>
-      </c>
-      <c r="E13" s="28">
-        <v>17</v>
-      </c>
-      <c r="F13" s="28">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6">
-      <c r="A14" s="28">
-        <v>14</v>
-      </c>
-      <c r="B14" s="28">
-        <v>15</v>
-      </c>
-      <c r="C14" s="28">
-        <v>16</v>
-      </c>
-      <c r="D14" s="28">
-        <v>17</v>
-      </c>
-      <c r="E14" s="28">
-        <v>18</v>
-      </c>
-      <c r="F14" s="28">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6">
-      <c r="A15" s="28">
-        <v>15</v>
-      </c>
-      <c r="B15" s="28">
-        <v>16</v>
-      </c>
-      <c r="C15" s="28">
-        <v>17</v>
-      </c>
-      <c r="D15" s="28">
-        <v>18</v>
-      </c>
-      <c r="E15" s="28">
-        <v>19</v>
-      </c>
-      <c r="F15" s="28">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6">
-      <c r="A16" s="28">
-        <v>16</v>
-      </c>
-      <c r="B16" s="28">
-        <v>17</v>
-      </c>
-      <c r="C16" s="28">
-        <v>18</v>
-      </c>
-      <c r="D16" s="28">
-        <v>19</v>
-      </c>
-      <c r="E16" s="28">
-        <v>20</v>
-      </c>
-      <c r="F16" s="28">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6">
-      <c r="A17" s="28">
-        <v>17</v>
-      </c>
-      <c r="B17" s="28">
-        <v>18</v>
-      </c>
-      <c r="C17" s="28">
-        <v>19</v>
-      </c>
-      <c r="D17" s="28">
-        <v>20</v>
-      </c>
-      <c r="E17" s="28">
-        <v>21</v>
-      </c>
-      <c r="F17" s="28">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6">
-      <c r="A18" s="28">
-        <v>18</v>
-      </c>
-      <c r="B18" s="28">
-        <v>19</v>
-      </c>
-      <c r="C18" s="28">
-        <v>20</v>
-      </c>
-      <c r="D18" s="28">
-        <v>21</v>
-      </c>
-      <c r="E18" s="28">
-        <v>22</v>
-      </c>
-      <c r="F18" s="28">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6">
-      <c r="A19" s="28">
-        <v>19</v>
-      </c>
-      <c r="B19" s="28">
-        <v>20</v>
-      </c>
-      <c r="C19" s="28">
-        <v>21</v>
-      </c>
-      <c r="D19" s="28">
-        <v>22</v>
-      </c>
-      <c r="E19" s="28">
-        <v>23</v>
-      </c>
-      <c r="F19" s="28">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6">
-      <c r="A20" s="28">
-        <v>20</v>
-      </c>
-      <c r="B20" s="28">
-        <v>21</v>
-      </c>
-      <c r="C20" s="28">
-        <v>22</v>
-      </c>
-      <c r="D20" s="28">
-        <v>23</v>
-      </c>
-      <c r="E20" s="28">
-        <v>24</v>
-      </c>
-      <c r="F20" s="28">
-        <v>25</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="11" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G8"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
@@ -1751,10 +1331,10 @@
       <c r="D1" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="29" t="s">
-        <v>11</v>
-      </c>
-      <c r="F1" s="29">
+      <c r="E1" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="28">
         <v>2.77</v>
       </c>
       <c r="G1" s="23" t="s">
@@ -1774,10 +1354,10 @@
       <c r="D2" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="29" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" s="29">
+      <c r="E2" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="28">
         <v>1.1200000000000001</v>
       </c>
       <c r="G2" s="23" t="s">
@@ -1797,10 +1377,10 @@
       <c r="D3" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="29" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3" s="29">
+      <c r="E3" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="28">
         <v>1.01</v>
       </c>
       <c r="G3" s="23" t="s">
@@ -1820,10 +1400,10 @@
       <c r="D4" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="29" t="s">
-        <v>11</v>
-      </c>
-      <c r="F4" s="29">
+      <c r="E4" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="28">
         <v>1.44</v>
       </c>
       <c r="G4" s="23" t="s">
@@ -1843,10 +1423,10 @@
       <c r="D5" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="29" t="s">
-        <v>11</v>
-      </c>
-      <c r="F5" s="29">
+      <c r="E5" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="28">
         <v>1.25</v>
       </c>
       <c r="G5" s="23" t="s">
@@ -1866,10 +1446,10 @@
       <c r="D6" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="29" t="s">
-        <v>11</v>
-      </c>
-      <c r="F6" s="29">
+      <c r="E6" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" s="28">
         <v>1.33</v>
       </c>
       <c r="G6" s="23" t="s">
@@ -1889,10 +1469,10 @@
       <c r="D7" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="E7" s="29" t="s">
-        <v>11</v>
-      </c>
-      <c r="F7" s="29">
+      <c r="E7" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7" s="28">
         <v>1.25</v>
       </c>
       <c r="G7" s="24" t="s">
@@ -1912,10 +1492,10 @@
       <c r="D8" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="E8" s="29" t="s">
-        <v>11</v>
-      </c>
-      <c r="F8" s="29">
+      <c r="E8" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="F8" s="28">
         <v>1.21</v>
       </c>
       <c r="G8" s="26" t="s">
@@ -1938,12 +1518,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -1958,15 +1538,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="33" customHeight="1">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
     </row>
     <row r="2" spans="1:7" ht="21" customHeight="1">
       <c r="A2" s="21" t="s">
@@ -2383,13 +1963,13 @@
       </c>
     </row>
     <row r="20" spans="1:7" ht="16.5">
-      <c r="A20" s="32"/>
-      <c r="B20" s="32"/>
-      <c r="C20" s="32"/>
-      <c r="D20" s="32"/>
-      <c r="E20" s="32"/>
-      <c r="F20" s="32"/>
-      <c r="G20" s="32"/>
+      <c r="A20" s="31"/>
+      <c r="B20" s="31"/>
+      <c r="C20" s="31"/>
+      <c r="D20" s="31"/>
+      <c r="E20" s="31"/>
+      <c r="F20" s="31"/>
+      <c r="G20" s="31"/>
     </row>
     <row r="21" spans="1:7" ht="16.5">
       <c r="A21" s="27"/>
@@ -2457,11 +2037,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A33" workbookViewId="0">
       <selection sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
@@ -2476,14 +2056,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="33.950000000000003" customHeight="1">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="32" t="s">
         <v>45</v>
       </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
     </row>
     <row r="2" spans="1:6" s="1" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A2" s="7" t="s">
@@ -3326,12 +2906,12 @@
       </c>
     </row>
     <row r="44" spans="1:6">
-      <c r="A44" s="34"/>
-      <c r="B44" s="34"/>
-      <c r="C44" s="34"/>
-      <c r="D44" s="35"/>
-      <c r="E44" s="34"/>
-      <c r="F44" s="34"/>
+      <c r="A44" s="33"/>
+      <c r="B44" s="33"/>
+      <c r="C44" s="33"/>
+      <c r="D44" s="34"/>
+      <c r="E44" s="33"/>
+      <c r="F44" s="33"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -3392,12 +2972,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G160"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:B17"/>
+    <sheetView tabSelected="1" topLeftCell="A109" workbookViewId="0">
+      <selection activeCell="J130" sqref="J130"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -3410,15 +2990,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="33" customHeight="1">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="50" t="s">
         <v>130</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="38"/>
+      <c r="B1" s="51"/>
+      <c r="C1" s="51"/>
+      <c r="D1" s="51"/>
+      <c r="E1" s="51"/>
+      <c r="F1" s="51"/>
+      <c r="G1" s="52"/>
     </row>
     <row r="2" spans="1:7" s="1" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A2" s="4" t="s">
@@ -3444,10 +3024,10 @@
       </c>
     </row>
     <row r="3" spans="1:7" ht="16.5">
-      <c r="A3" s="39">
+      <c r="A3" s="38">
         <v>1</v>
       </c>
-      <c r="B3" s="54" t="s">
+      <c r="B3" s="46" t="s">
         <v>137</v>
       </c>
       <c r="C3" s="7" t="s">
@@ -3459,16 +3039,16 @@
       <c r="E3" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="43" t="s">
+      <c r="F3" s="54" t="s">
         <v>18</v>
       </c>
-      <c r="G3" s="39">
+      <c r="G3" s="38">
         <v>1.83</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="16.5">
-      <c r="A4" s="39"/>
-      <c r="B4" s="54"/>
+      <c r="A4" s="38"/>
+      <c r="B4" s="46"/>
       <c r="C4" s="7" t="s">
         <v>139</v>
       </c>
@@ -3478,12 +3058,12 @@
       <c r="E4" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F4" s="44"/>
-      <c r="G4" s="39"/>
+      <c r="F4" s="55"/>
+      <c r="G4" s="38"/>
     </row>
     <row r="5" spans="1:7" ht="16.5">
-      <c r="A5" s="39"/>
-      <c r="B5" s="54"/>
+      <c r="A5" s="38"/>
+      <c r="B5" s="46"/>
       <c r="C5" s="7" t="s">
         <v>140</v>
       </c>
@@ -3493,12 +3073,12 @@
       <c r="E5" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F5" s="44"/>
-      <c r="G5" s="39"/>
+      <c r="F5" s="55"/>
+      <c r="G5" s="38"/>
     </row>
     <row r="6" spans="1:7" ht="16.5">
-      <c r="A6" s="39"/>
-      <c r="B6" s="54"/>
+      <c r="A6" s="38"/>
+      <c r="B6" s="46"/>
       <c r="C6" s="7" t="s">
         <v>141</v>
       </c>
@@ -3508,12 +3088,12 @@
       <c r="E6" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F6" s="44"/>
-      <c r="G6" s="39"/>
+      <c r="F6" s="55"/>
+      <c r="G6" s="38"/>
     </row>
     <row r="7" spans="1:7" ht="16.5">
-      <c r="A7" s="39"/>
-      <c r="B7" s="54"/>
+      <c r="A7" s="38"/>
+      <c r="B7" s="46"/>
       <c r="C7" s="7" t="s">
         <v>142</v>
       </c>
@@ -3523,12 +3103,12 @@
       <c r="E7" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F7" s="44"/>
-      <c r="G7" s="39"/>
+      <c r="F7" s="55"/>
+      <c r="G7" s="38"/>
     </row>
     <row r="8" spans="1:7" ht="16.5">
-      <c r="A8" s="39"/>
-      <c r="B8" s="54"/>
+      <c r="A8" s="38"/>
+      <c r="B8" s="46"/>
       <c r="C8" s="7" t="s">
         <v>143</v>
       </c>
@@ -3538,12 +3118,12 @@
       <c r="E8" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F8" s="44"/>
-      <c r="G8" s="39"/>
+      <c r="F8" s="55"/>
+      <c r="G8" s="38"/>
     </row>
     <row r="9" spans="1:7" ht="16.5">
-      <c r="A9" s="39"/>
-      <c r="B9" s="54"/>
+      <c r="A9" s="38"/>
+      <c r="B9" s="46"/>
       <c r="C9" s="7" t="s">
         <v>144</v>
       </c>
@@ -3553,12 +3133,12 @@
       <c r="E9" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F9" s="44"/>
-      <c r="G9" s="39"/>
+      <c r="F9" s="55"/>
+      <c r="G9" s="38"/>
     </row>
     <row r="10" spans="1:7" ht="16.5">
-      <c r="A10" s="39"/>
-      <c r="B10" s="54"/>
+      <c r="A10" s="38"/>
+      <c r="B10" s="46"/>
       <c r="C10" s="7" t="s">
         <v>145</v>
       </c>
@@ -3568,12 +3148,12 @@
       <c r="E10" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F10" s="44"/>
-      <c r="G10" s="39"/>
+      <c r="F10" s="55"/>
+      <c r="G10" s="38"/>
     </row>
     <row r="11" spans="1:7" ht="16.5">
-      <c r="A11" s="39"/>
-      <c r="B11" s="54"/>
+      <c r="A11" s="38"/>
+      <c r="B11" s="46"/>
       <c r="C11" s="4" t="s">
         <v>146</v>
       </c>
@@ -3583,12 +3163,12 @@
       <c r="E11" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F11" s="44"/>
-      <c r="G11" s="39"/>
+      <c r="F11" s="55"/>
+      <c r="G11" s="38"/>
     </row>
     <row r="12" spans="1:7" ht="16.5">
-      <c r="A12" s="39"/>
-      <c r="B12" s="54"/>
+      <c r="A12" s="38"/>
+      <c r="B12" s="46"/>
       <c r="C12" s="4" t="s">
         <v>147</v>
       </c>
@@ -3598,12 +3178,12 @@
       <c r="E12" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F12" s="44"/>
-      <c r="G12" s="39"/>
+      <c r="F12" s="55"/>
+      <c r="G12" s="38"/>
     </row>
     <row r="13" spans="1:7" ht="16.5">
-      <c r="A13" s="39"/>
-      <c r="B13" s="54"/>
+      <c r="A13" s="38"/>
+      <c r="B13" s="46"/>
       <c r="C13" s="4" t="s">
         <v>148</v>
       </c>
@@ -3613,12 +3193,12 @@
       <c r="E13" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F13" s="44"/>
-      <c r="G13" s="39"/>
+      <c r="F13" s="55"/>
+      <c r="G13" s="38"/>
     </row>
     <row r="14" spans="1:7" ht="16.5">
-      <c r="A14" s="39"/>
-      <c r="B14" s="54"/>
+      <c r="A14" s="38"/>
+      <c r="B14" s="46"/>
       <c r="C14" s="7" t="s">
         <v>149</v>
       </c>
@@ -3628,12 +3208,12 @@
       <c r="E14" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F14" s="44"/>
-      <c r="G14" s="39"/>
+      <c r="F14" s="55"/>
+      <c r="G14" s="38"/>
     </row>
     <row r="15" spans="1:7" ht="16.5">
-      <c r="A15" s="39"/>
-      <c r="B15" s="54"/>
+      <c r="A15" s="38"/>
+      <c r="B15" s="46"/>
       <c r="C15" s="7" t="s">
         <v>150</v>
       </c>
@@ -3643,12 +3223,12 @@
       <c r="E15" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F15" s="44"/>
-      <c r="G15" s="39"/>
+      <c r="F15" s="55"/>
+      <c r="G15" s="38"/>
     </row>
     <row r="16" spans="1:7" ht="16.5">
-      <c r="A16" s="39"/>
-      <c r="B16" s="54"/>
+      <c r="A16" s="38"/>
+      <c r="B16" s="46"/>
       <c r="C16" s="4" t="s">
         <v>151</v>
       </c>
@@ -3658,12 +3238,12 @@
       <c r="E16" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F16" s="44"/>
-      <c r="G16" s="39"/>
+      <c r="F16" s="55"/>
+      <c r="G16" s="38"/>
     </row>
     <row r="17" spans="1:7" ht="16.5">
-      <c r="A17" s="40"/>
-      <c r="B17" s="55"/>
+      <c r="A17" s="53"/>
+      <c r="B17" s="47"/>
       <c r="C17" s="4" t="s">
         <v>152</v>
       </c>
@@ -3673,14 +3253,14 @@
       <c r="E17" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F17" s="45"/>
-      <c r="G17" s="39"/>
+      <c r="F17" s="56"/>
+      <c r="G17" s="38"/>
     </row>
     <row r="18" spans="1:7" ht="18.95" customHeight="1">
-      <c r="A18" s="41">
+      <c r="A18" s="39">
         <v>2</v>
       </c>
-      <c r="B18" s="50" t="s">
+      <c r="B18" s="48" t="s">
         <v>153</v>
       </c>
       <c r="C18" s="7" t="s">
@@ -3692,16 +3272,16 @@
       <c r="E18" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F18" s="46" t="s">
+      <c r="F18" s="57" t="s">
         <v>16</v>
       </c>
-      <c r="G18" s="41">
+      <c r="G18" s="39">
         <v>1.1299999999999999</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="16.5">
-      <c r="A19" s="41"/>
-      <c r="B19" s="50"/>
+      <c r="A19" s="39"/>
+      <c r="B19" s="48"/>
       <c r="C19" s="7" t="s">
         <v>139</v>
       </c>
@@ -3711,12 +3291,12 @@
       <c r="E19" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F19" s="47"/>
-      <c r="G19" s="41"/>
+      <c r="F19" s="58"/>
+      <c r="G19" s="39"/>
     </row>
     <row r="20" spans="1:7" ht="16.5">
-      <c r="A20" s="41"/>
-      <c r="B20" s="50"/>
+      <c r="A20" s="39"/>
+      <c r="B20" s="48"/>
       <c r="C20" s="7" t="s">
         <v>140</v>
       </c>
@@ -3726,12 +3306,12 @@
       <c r="E20" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F20" s="47"/>
-      <c r="G20" s="41"/>
+      <c r="F20" s="58"/>
+      <c r="G20" s="39"/>
     </row>
     <row r="21" spans="1:7" ht="16.5">
-      <c r="A21" s="41"/>
-      <c r="B21" s="50"/>
+      <c r="A21" s="39"/>
+      <c r="B21" s="48"/>
       <c r="C21" s="7" t="s">
         <v>141</v>
       </c>
@@ -3741,12 +3321,12 @@
       <c r="E21" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F21" s="47"/>
-      <c r="G21" s="41"/>
+      <c r="F21" s="58"/>
+      <c r="G21" s="39"/>
     </row>
     <row r="22" spans="1:7" ht="16.5">
-      <c r="A22" s="41"/>
-      <c r="B22" s="50"/>
+      <c r="A22" s="39"/>
+      <c r="B22" s="48"/>
       <c r="C22" s="7" t="s">
         <v>142</v>
       </c>
@@ -3756,12 +3336,12 @@
       <c r="E22" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F22" s="47"/>
-      <c r="G22" s="41"/>
+      <c r="F22" s="58"/>
+      <c r="G22" s="39"/>
     </row>
     <row r="23" spans="1:7" ht="16.5">
-      <c r="A23" s="41"/>
-      <c r="B23" s="50"/>
+      <c r="A23" s="39"/>
+      <c r="B23" s="48"/>
       <c r="C23" s="7" t="s">
         <v>143</v>
       </c>
@@ -3771,12 +3351,12 @@
       <c r="E23" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F23" s="47"/>
-      <c r="G23" s="41"/>
+      <c r="F23" s="58"/>
+      <c r="G23" s="39"/>
     </row>
     <row r="24" spans="1:7" ht="16.5">
-      <c r="A24" s="41"/>
-      <c r="B24" s="50"/>
+      <c r="A24" s="39"/>
+      <c r="B24" s="48"/>
       <c r="C24" s="7" t="s">
         <v>144</v>
       </c>
@@ -3786,12 +3366,12 @@
       <c r="E24" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F24" s="47"/>
-      <c r="G24" s="41"/>
+      <c r="F24" s="58"/>
+      <c r="G24" s="39"/>
     </row>
     <row r="25" spans="1:7" ht="16.5">
-      <c r="A25" s="41"/>
-      <c r="B25" s="50"/>
+      <c r="A25" s="39"/>
+      <c r="B25" s="48"/>
       <c r="C25" s="7" t="s">
         <v>145</v>
       </c>
@@ -3801,12 +3381,12 @@
       <c r="E25" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F25" s="47"/>
-      <c r="G25" s="41"/>
+      <c r="F25" s="58"/>
+      <c r="G25" s="39"/>
     </row>
     <row r="26" spans="1:7" ht="16.5">
-      <c r="A26" s="41"/>
-      <c r="B26" s="50"/>
+      <c r="A26" s="39"/>
+      <c r="B26" s="48"/>
       <c r="C26" s="7" t="s">
         <v>149</v>
       </c>
@@ -3816,12 +3396,12 @@
       <c r="E26" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F26" s="47"/>
-      <c r="G26" s="41"/>
+      <c r="F26" s="58"/>
+      <c r="G26" s="39"/>
     </row>
     <row r="27" spans="1:7" ht="16.5">
-      <c r="A27" s="41"/>
-      <c r="B27" s="50"/>
+      <c r="A27" s="39"/>
+      <c r="B27" s="48"/>
       <c r="C27" s="7" t="s">
         <v>150</v>
       </c>
@@ -3831,12 +3411,12 @@
       <c r="E27" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F27" s="47"/>
-      <c r="G27" s="41"/>
+      <c r="F27" s="58"/>
+      <c r="G27" s="39"/>
     </row>
     <row r="28" spans="1:7" ht="16.5">
-      <c r="A28" s="41"/>
-      <c r="B28" s="50"/>
+      <c r="A28" s="39"/>
+      <c r="B28" s="48"/>
       <c r="C28" s="7" t="s">
         <v>154</v>
       </c>
@@ -3846,12 +3426,12 @@
       <c r="E28" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F28" s="47"/>
-      <c r="G28" s="41"/>
+      <c r="F28" s="58"/>
+      <c r="G28" s="39"/>
     </row>
     <row r="29" spans="1:7" ht="16.5">
-      <c r="A29" s="41"/>
-      <c r="B29" s="50"/>
+      <c r="A29" s="39"/>
+      <c r="B29" s="48"/>
       <c r="C29" s="7" t="s">
         <v>155</v>
       </c>
@@ -3861,12 +3441,12 @@
       <c r="E29" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F29" s="47"/>
-      <c r="G29" s="41"/>
+      <c r="F29" s="58"/>
+      <c r="G29" s="39"/>
     </row>
     <row r="30" spans="1:7" ht="16.5">
-      <c r="A30" s="42"/>
-      <c r="B30" s="51"/>
+      <c r="A30" s="40"/>
+      <c r="B30" s="49"/>
       <c r="C30" s="9" t="s">
         <v>156</v>
       </c>
@@ -3876,14 +3456,14 @@
       <c r="E30" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="F30" s="48"/>
-      <c r="G30" s="42"/>
+      <c r="F30" s="59"/>
+      <c r="G30" s="40"/>
     </row>
     <row r="31" spans="1:7" ht="16.5">
-      <c r="A31" s="41">
+      <c r="A31" s="39">
         <v>3</v>
       </c>
-      <c r="B31" s="50" t="s">
+      <c r="B31" s="48" t="s">
         <v>157</v>
       </c>
       <c r="C31" s="7" t="s">
@@ -3895,16 +3475,16 @@
       <c r="E31" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F31" s="49" t="s">
+      <c r="F31" s="60" t="s">
         <v>158</v>
       </c>
-      <c r="G31" s="41">
+      <c r="G31" s="39">
         <v>1.2</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="16.5">
-      <c r="A32" s="41"/>
-      <c r="B32" s="50"/>
+      <c r="A32" s="39"/>
+      <c r="B32" s="48"/>
       <c r="C32" s="7" t="s">
         <v>139</v>
       </c>
@@ -3914,12 +3494,12 @@
       <c r="E32" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F32" s="50"/>
-      <c r="G32" s="41"/>
+      <c r="F32" s="48"/>
+      <c r="G32" s="39"/>
     </row>
     <row r="33" spans="1:7" ht="16.5">
-      <c r="A33" s="41"/>
-      <c r="B33" s="50"/>
+      <c r="A33" s="39"/>
+      <c r="B33" s="48"/>
       <c r="C33" s="7" t="s">
         <v>140</v>
       </c>
@@ -3929,12 +3509,12 @@
       <c r="E33" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F33" s="50"/>
-      <c r="G33" s="41"/>
+      <c r="F33" s="48"/>
+      <c r="G33" s="39"/>
     </row>
     <row r="34" spans="1:7" ht="16.5">
-      <c r="A34" s="41"/>
-      <c r="B34" s="50"/>
+      <c r="A34" s="39"/>
+      <c r="B34" s="48"/>
       <c r="C34" s="7" t="s">
         <v>141</v>
       </c>
@@ -3944,12 +3524,12 @@
       <c r="E34" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F34" s="50"/>
-      <c r="G34" s="41"/>
+      <c r="F34" s="48"/>
+      <c r="G34" s="39"/>
     </row>
     <row r="35" spans="1:7" ht="16.5">
-      <c r="A35" s="41"/>
-      <c r="B35" s="50"/>
+      <c r="A35" s="39"/>
+      <c r="B35" s="48"/>
       <c r="C35" s="7" t="s">
         <v>142</v>
       </c>
@@ -3959,12 +3539,12 @@
       <c r="E35" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F35" s="50"/>
-      <c r="G35" s="41"/>
+      <c r="F35" s="48"/>
+      <c r="G35" s="39"/>
     </row>
     <row r="36" spans="1:7" ht="16.5">
-      <c r="A36" s="41"/>
-      <c r="B36" s="50"/>
+      <c r="A36" s="39"/>
+      <c r="B36" s="48"/>
       <c r="C36" s="7" t="s">
         <v>143</v>
       </c>
@@ -3974,12 +3554,12 @@
       <c r="E36" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F36" s="50"/>
-      <c r="G36" s="41"/>
+      <c r="F36" s="48"/>
+      <c r="G36" s="39"/>
     </row>
     <row r="37" spans="1:7" ht="16.5">
-      <c r="A37" s="41"/>
-      <c r="B37" s="50"/>
+      <c r="A37" s="39"/>
+      <c r="B37" s="48"/>
       <c r="C37" s="7" t="s">
         <v>144</v>
       </c>
@@ -3989,12 +3569,12 @@
       <c r="E37" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F37" s="50"/>
-      <c r="G37" s="41"/>
+      <c r="F37" s="48"/>
+      <c r="G37" s="39"/>
     </row>
     <row r="38" spans="1:7" ht="16.5">
-      <c r="A38" s="41"/>
-      <c r="B38" s="50"/>
+      <c r="A38" s="39"/>
+      <c r="B38" s="48"/>
       <c r="C38" s="7" t="s">
         <v>145</v>
       </c>
@@ -4004,12 +3584,12 @@
       <c r="E38" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F38" s="50"/>
-      <c r="G38" s="41"/>
+      <c r="F38" s="48"/>
+      <c r="G38" s="39"/>
     </row>
     <row r="39" spans="1:7" ht="16.5">
-      <c r="A39" s="41"/>
-      <c r="B39" s="50"/>
+      <c r="A39" s="39"/>
+      <c r="B39" s="48"/>
       <c r="C39" s="7" t="s">
         <v>149</v>
       </c>
@@ -4019,12 +3599,12 @@
       <c r="E39" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F39" s="50"/>
-      <c r="G39" s="41"/>
+      <c r="F39" s="48"/>
+      <c r="G39" s="39"/>
     </row>
     <row r="40" spans="1:7" ht="16.5">
-      <c r="A40" s="41"/>
-      <c r="B40" s="50"/>
+      <c r="A40" s="39"/>
+      <c r="B40" s="48"/>
       <c r="C40" s="7" t="s">
         <v>150</v>
       </c>
@@ -4034,12 +3614,12 @@
       <c r="E40" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F40" s="50"/>
-      <c r="G40" s="41"/>
+      <c r="F40" s="48"/>
+      <c r="G40" s="39"/>
     </row>
     <row r="41" spans="1:7" ht="16.5">
-      <c r="A41" s="41"/>
-      <c r="B41" s="50"/>
+      <c r="A41" s="39"/>
+      <c r="B41" s="48"/>
       <c r="C41" s="7" t="s">
         <v>154</v>
       </c>
@@ -4049,12 +3629,12 @@
       <c r="E41" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F41" s="50"/>
-      <c r="G41" s="41"/>
+      <c r="F41" s="48"/>
+      <c r="G41" s="39"/>
     </row>
     <row r="42" spans="1:7" ht="16.5">
-      <c r="A42" s="41"/>
-      <c r="B42" s="50"/>
+      <c r="A42" s="39"/>
+      <c r="B42" s="48"/>
       <c r="C42" s="7" t="s">
         <v>155</v>
       </c>
@@ -4064,12 +3644,12 @@
       <c r="E42" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F42" s="50"/>
-      <c r="G42" s="41"/>
+      <c r="F42" s="48"/>
+      <c r="G42" s="39"/>
     </row>
     <row r="43" spans="1:7" ht="16.5">
-      <c r="A43" s="42"/>
-      <c r="B43" s="51"/>
+      <c r="A43" s="40"/>
+      <c r="B43" s="49"/>
       <c r="C43" s="9" t="s">
         <v>156</v>
       </c>
@@ -4079,14 +3659,14 @@
       <c r="E43" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="F43" s="51"/>
-      <c r="G43" s="42"/>
+      <c r="F43" s="49"/>
+      <c r="G43" s="40"/>
     </row>
     <row r="44" spans="1:7" ht="16.5">
-      <c r="A44" s="41">
+      <c r="A44" s="39">
         <v>4</v>
       </c>
-      <c r="B44" s="50" t="s">
+      <c r="B44" s="48" t="s">
         <v>159</v>
       </c>
       <c r="C44" s="7" t="s">
@@ -4098,16 +3678,16 @@
       <c r="E44" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F44" s="52" t="s">
+      <c r="F44" s="61" t="s">
         <v>160</v>
       </c>
-      <c r="G44" s="41">
+      <c r="G44" s="39">
         <v>1.05</v>
       </c>
     </row>
     <row r="45" spans="1:7" ht="16.5">
-      <c r="A45" s="41"/>
-      <c r="B45" s="50"/>
+      <c r="A45" s="39"/>
+      <c r="B45" s="48"/>
       <c r="C45" s="7" t="s">
         <v>139</v>
       </c>
@@ -4117,12 +3697,12 @@
       <c r="E45" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F45" s="53"/>
-      <c r="G45" s="41"/>
+      <c r="F45" s="36"/>
+      <c r="G45" s="39"/>
     </row>
     <row r="46" spans="1:7" ht="16.5">
-      <c r="A46" s="41"/>
-      <c r="B46" s="50"/>
+      <c r="A46" s="39"/>
+      <c r="B46" s="48"/>
       <c r="C46" s="7" t="s">
         <v>140</v>
       </c>
@@ -4132,12 +3712,12 @@
       <c r="E46" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F46" s="53"/>
-      <c r="G46" s="41"/>
+      <c r="F46" s="36"/>
+      <c r="G46" s="39"/>
     </row>
     <row r="47" spans="1:7" ht="16.5">
-      <c r="A47" s="41"/>
-      <c r="B47" s="50"/>
+      <c r="A47" s="39"/>
+      <c r="B47" s="48"/>
       <c r="C47" s="7" t="s">
         <v>141</v>
       </c>
@@ -4147,12 +3727,12 @@
       <c r="E47" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F47" s="53"/>
-      <c r="G47" s="41"/>
+      <c r="F47" s="36"/>
+      <c r="G47" s="39"/>
     </row>
     <row r="48" spans="1:7" ht="16.5">
-      <c r="A48" s="41"/>
-      <c r="B48" s="50"/>
+      <c r="A48" s="39"/>
+      <c r="B48" s="48"/>
       <c r="C48" s="7" t="s">
         <v>142</v>
       </c>
@@ -4162,12 +3742,12 @@
       <c r="E48" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F48" s="53"/>
-      <c r="G48" s="41"/>
+      <c r="F48" s="36"/>
+      <c r="G48" s="39"/>
     </row>
     <row r="49" spans="1:7" ht="16.5">
-      <c r="A49" s="41"/>
-      <c r="B49" s="50"/>
+      <c r="A49" s="39"/>
+      <c r="B49" s="48"/>
       <c r="C49" s="7" t="s">
         <v>143</v>
       </c>
@@ -4177,12 +3757,12 @@
       <c r="E49" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F49" s="53"/>
-      <c r="G49" s="41"/>
+      <c r="F49" s="36"/>
+      <c r="G49" s="39"/>
     </row>
     <row r="50" spans="1:7" ht="16.5">
-      <c r="A50" s="41"/>
-      <c r="B50" s="50"/>
+      <c r="A50" s="39"/>
+      <c r="B50" s="48"/>
       <c r="C50" s="7" t="s">
         <v>144</v>
       </c>
@@ -4192,12 +3772,12 @@
       <c r="E50" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F50" s="53"/>
-      <c r="G50" s="41"/>
+      <c r="F50" s="36"/>
+      <c r="G50" s="39"/>
     </row>
     <row r="51" spans="1:7" ht="16.5">
-      <c r="A51" s="41"/>
-      <c r="B51" s="50"/>
+      <c r="A51" s="39"/>
+      <c r="B51" s="48"/>
       <c r="C51" s="7" t="s">
         <v>145</v>
       </c>
@@ -4207,12 +3787,12 @@
       <c r="E51" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F51" s="53"/>
-      <c r="G51" s="41"/>
+      <c r="F51" s="36"/>
+      <c r="G51" s="39"/>
     </row>
     <row r="52" spans="1:7" ht="16.5">
-      <c r="A52" s="41"/>
-      <c r="B52" s="50"/>
+      <c r="A52" s="39"/>
+      <c r="B52" s="48"/>
       <c r="C52" s="7" t="s">
         <v>149</v>
       </c>
@@ -4222,12 +3802,12 @@
       <c r="E52" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F52" s="53"/>
-      <c r="G52" s="41"/>
+      <c r="F52" s="36"/>
+      <c r="G52" s="39"/>
     </row>
     <row r="53" spans="1:7" ht="16.5">
-      <c r="A53" s="41"/>
-      <c r="B53" s="50"/>
+      <c r="A53" s="39"/>
+      <c r="B53" s="48"/>
       <c r="C53" s="7" t="s">
         <v>150</v>
       </c>
@@ -4237,12 +3817,12 @@
       <c r="E53" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F53" s="53"/>
-      <c r="G53" s="41"/>
+      <c r="F53" s="36"/>
+      <c r="G53" s="39"/>
     </row>
     <row r="54" spans="1:7" ht="16.5">
-      <c r="A54" s="41"/>
-      <c r="B54" s="50"/>
+      <c r="A54" s="39"/>
+      <c r="B54" s="48"/>
       <c r="C54" s="7" t="s">
         <v>154</v>
       </c>
@@ -4252,12 +3832,12 @@
       <c r="E54" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F54" s="53"/>
-      <c r="G54" s="41"/>
+      <c r="F54" s="36"/>
+      <c r="G54" s="39"/>
     </row>
     <row r="55" spans="1:7" ht="16.5">
-      <c r="A55" s="41"/>
-      <c r="B55" s="50"/>
+      <c r="A55" s="39"/>
+      <c r="B55" s="48"/>
       <c r="C55" s="7" t="s">
         <v>155</v>
       </c>
@@ -4267,12 +3847,12 @@
       <c r="E55" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F55" s="53"/>
-      <c r="G55" s="41"/>
+      <c r="F55" s="36"/>
+      <c r="G55" s="39"/>
     </row>
     <row r="56" spans="1:7" ht="16.5">
-      <c r="A56" s="41"/>
-      <c r="B56" s="50"/>
+      <c r="A56" s="39"/>
+      <c r="B56" s="48"/>
       <c r="C56" s="7" t="s">
         <v>156</v>
       </c>
@@ -4282,14 +3862,14 @@
       <c r="E56" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F56" s="53"/>
-      <c r="G56" s="41"/>
+      <c r="F56" s="36"/>
+      <c r="G56" s="39"/>
     </row>
     <row r="57" spans="1:7" ht="16.5">
-      <c r="A57" s="41">
+      <c r="A57" s="39">
         <v>5</v>
       </c>
-      <c r="B57" s="50" t="s">
+      <c r="B57" s="48" t="s">
         <v>161</v>
       </c>
       <c r="C57" s="7" t="s">
@@ -4301,16 +3881,16 @@
       <c r="E57" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F57" s="58" t="s">
+      <c r="F57" s="35" t="s">
         <v>162</v>
       </c>
-      <c r="G57" s="41">
+      <c r="G57" s="39">
         <v>0.98</v>
       </c>
     </row>
     <row r="58" spans="1:7" ht="16.5">
-      <c r="A58" s="41"/>
-      <c r="B58" s="50"/>
+      <c r="A58" s="39"/>
+      <c r="B58" s="48"/>
       <c r="C58" s="7" t="s">
         <v>139</v>
       </c>
@@ -4320,12 +3900,12 @@
       <c r="E58" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F58" s="53"/>
-      <c r="G58" s="41"/>
+      <c r="F58" s="36"/>
+      <c r="G58" s="39"/>
     </row>
     <row r="59" spans="1:7" ht="16.5">
-      <c r="A59" s="41"/>
-      <c r="B59" s="50"/>
+      <c r="A59" s="39"/>
+      <c r="B59" s="48"/>
       <c r="C59" s="7" t="s">
         <v>140</v>
       </c>
@@ -4335,12 +3915,12 @@
       <c r="E59" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F59" s="53"/>
-      <c r="G59" s="41"/>
+      <c r="F59" s="36"/>
+      <c r="G59" s="39"/>
     </row>
     <row r="60" spans="1:7" ht="16.5">
-      <c r="A60" s="41"/>
-      <c r="B60" s="50"/>
+      <c r="A60" s="39"/>
+      <c r="B60" s="48"/>
       <c r="C60" s="7" t="s">
         <v>141</v>
       </c>
@@ -4350,12 +3930,12 @@
       <c r="E60" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F60" s="53"/>
-      <c r="G60" s="41"/>
+      <c r="F60" s="36"/>
+      <c r="G60" s="39"/>
     </row>
     <row r="61" spans="1:7" ht="16.5">
-      <c r="A61" s="41"/>
-      <c r="B61" s="50"/>
+      <c r="A61" s="39"/>
+      <c r="B61" s="48"/>
       <c r="C61" s="7" t="s">
         <v>142</v>
       </c>
@@ -4365,12 +3945,12 @@
       <c r="E61" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F61" s="53"/>
-      <c r="G61" s="41"/>
+      <c r="F61" s="36"/>
+      <c r="G61" s="39"/>
     </row>
     <row r="62" spans="1:7" ht="16.5">
-      <c r="A62" s="41"/>
-      <c r="B62" s="50"/>
+      <c r="A62" s="39"/>
+      <c r="B62" s="48"/>
       <c r="C62" s="7" t="s">
         <v>143</v>
       </c>
@@ -4380,12 +3960,12 @@
       <c r="E62" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F62" s="53"/>
-      <c r="G62" s="41"/>
+      <c r="F62" s="36"/>
+      <c r="G62" s="39"/>
     </row>
     <row r="63" spans="1:7" ht="16.5">
-      <c r="A63" s="41"/>
-      <c r="B63" s="50"/>
+      <c r="A63" s="39"/>
+      <c r="B63" s="48"/>
       <c r="C63" s="7" t="s">
         <v>144</v>
       </c>
@@ -4395,12 +3975,12 @@
       <c r="E63" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F63" s="53"/>
-      <c r="G63" s="41"/>
+      <c r="F63" s="36"/>
+      <c r="G63" s="39"/>
     </row>
     <row r="64" spans="1:7" ht="16.5">
-      <c r="A64" s="41"/>
-      <c r="B64" s="50"/>
+      <c r="A64" s="39"/>
+      <c r="B64" s="48"/>
       <c r="C64" s="7" t="s">
         <v>145</v>
       </c>
@@ -4410,12 +3990,12 @@
       <c r="E64" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F64" s="53"/>
-      <c r="G64" s="41"/>
+      <c r="F64" s="36"/>
+      <c r="G64" s="39"/>
     </row>
     <row r="65" spans="1:7" ht="16.5">
-      <c r="A65" s="41"/>
-      <c r="B65" s="50"/>
+      <c r="A65" s="39"/>
+      <c r="B65" s="48"/>
       <c r="C65" s="7" t="s">
         <v>149</v>
       </c>
@@ -4425,12 +4005,12 @@
       <c r="E65" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F65" s="53"/>
-      <c r="G65" s="41"/>
+      <c r="F65" s="36"/>
+      <c r="G65" s="39"/>
     </row>
     <row r="66" spans="1:7" ht="16.5">
-      <c r="A66" s="41"/>
-      <c r="B66" s="50"/>
+      <c r="A66" s="39"/>
+      <c r="B66" s="48"/>
       <c r="C66" s="7" t="s">
         <v>150</v>
       </c>
@@ -4440,12 +4020,12 @@
       <c r="E66" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F66" s="53"/>
-      <c r="G66" s="41"/>
+      <c r="F66" s="36"/>
+      <c r="G66" s="39"/>
     </row>
     <row r="67" spans="1:7" ht="16.5">
-      <c r="A67" s="41"/>
-      <c r="B67" s="50"/>
+      <c r="A67" s="39"/>
+      <c r="B67" s="48"/>
       <c r="C67" s="7" t="s">
         <v>154</v>
       </c>
@@ -4455,12 +4035,12 @@
       <c r="E67" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F67" s="53"/>
-      <c r="G67" s="41"/>
+      <c r="F67" s="36"/>
+      <c r="G67" s="39"/>
     </row>
     <row r="68" spans="1:7" ht="16.5">
-      <c r="A68" s="41"/>
-      <c r="B68" s="50"/>
+      <c r="A68" s="39"/>
+      <c r="B68" s="48"/>
       <c r="C68" s="7" t="s">
         <v>155</v>
       </c>
@@ -4470,12 +4050,12 @@
       <c r="E68" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F68" s="53"/>
-      <c r="G68" s="41"/>
+      <c r="F68" s="36"/>
+      <c r="G68" s="39"/>
     </row>
     <row r="69" spans="1:7" ht="16.5">
-      <c r="A69" s="42"/>
-      <c r="B69" s="51"/>
+      <c r="A69" s="40"/>
+      <c r="B69" s="49"/>
       <c r="C69" s="9" t="s">
         <v>156</v>
       </c>
@@ -4485,14 +4065,14 @@
       <c r="E69" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="F69" s="59"/>
-      <c r="G69" s="42"/>
+      <c r="F69" s="37"/>
+      <c r="G69" s="40"/>
     </row>
     <row r="70" spans="1:7" ht="16.5">
-      <c r="A70" s="41">
+      <c r="A70" s="39">
         <v>6</v>
       </c>
-      <c r="B70" s="50" t="s">
+      <c r="B70" s="48" t="s">
         <v>163</v>
       </c>
       <c r="C70" s="7" t="s">
@@ -4504,16 +4084,16 @@
       <c r="E70" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F70" s="58" t="s">
+      <c r="F70" s="35" t="s">
         <v>164</v>
       </c>
-      <c r="G70" s="41">
+      <c r="G70" s="39">
         <v>1.01</v>
       </c>
     </row>
     <row r="71" spans="1:7" ht="16.5">
-      <c r="A71" s="41"/>
-      <c r="B71" s="50"/>
+      <c r="A71" s="39"/>
+      <c r="B71" s="48"/>
       <c r="C71" s="7" t="s">
         <v>139</v>
       </c>
@@ -4523,12 +4103,12 @@
       <c r="E71" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F71" s="53"/>
-      <c r="G71" s="41"/>
+      <c r="F71" s="36"/>
+      <c r="G71" s="39"/>
     </row>
     <row r="72" spans="1:7" ht="16.5">
-      <c r="A72" s="41"/>
-      <c r="B72" s="50"/>
+      <c r="A72" s="39"/>
+      <c r="B72" s="48"/>
       <c r="C72" s="7" t="s">
         <v>140</v>
       </c>
@@ -4538,12 +4118,12 @@
       <c r="E72" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F72" s="53"/>
-      <c r="G72" s="41"/>
+      <c r="F72" s="36"/>
+      <c r="G72" s="39"/>
     </row>
     <row r="73" spans="1:7" ht="16.5">
-      <c r="A73" s="41"/>
-      <c r="B73" s="50"/>
+      <c r="A73" s="39"/>
+      <c r="B73" s="48"/>
       <c r="C73" s="7" t="s">
         <v>141</v>
       </c>
@@ -4553,12 +4133,12 @@
       <c r="E73" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F73" s="53"/>
-      <c r="G73" s="41"/>
+      <c r="F73" s="36"/>
+      <c r="G73" s="39"/>
     </row>
     <row r="74" spans="1:7" ht="16.5">
-      <c r="A74" s="41"/>
-      <c r="B74" s="50"/>
+      <c r="A74" s="39"/>
+      <c r="B74" s="48"/>
       <c r="C74" s="7" t="s">
         <v>142</v>
       </c>
@@ -4568,12 +4148,12 @@
       <c r="E74" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F74" s="53"/>
-      <c r="G74" s="41"/>
+      <c r="F74" s="36"/>
+      <c r="G74" s="39"/>
     </row>
     <row r="75" spans="1:7" ht="16.5">
-      <c r="A75" s="41"/>
-      <c r="B75" s="50"/>
+      <c r="A75" s="39"/>
+      <c r="B75" s="48"/>
       <c r="C75" s="7" t="s">
         <v>143</v>
       </c>
@@ -4583,12 +4163,12 @@
       <c r="E75" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F75" s="53"/>
-      <c r="G75" s="41"/>
+      <c r="F75" s="36"/>
+      <c r="G75" s="39"/>
     </row>
     <row r="76" spans="1:7" ht="16.5">
-      <c r="A76" s="41"/>
-      <c r="B76" s="50"/>
+      <c r="A76" s="39"/>
+      <c r="B76" s="48"/>
       <c r="C76" s="7" t="s">
         <v>144</v>
       </c>
@@ -4598,12 +4178,12 @@
       <c r="E76" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F76" s="53"/>
-      <c r="G76" s="41"/>
+      <c r="F76" s="36"/>
+      <c r="G76" s="39"/>
     </row>
     <row r="77" spans="1:7" ht="16.5">
-      <c r="A77" s="41"/>
-      <c r="B77" s="50"/>
+      <c r="A77" s="39"/>
+      <c r="B77" s="48"/>
       <c r="C77" s="7" t="s">
         <v>145</v>
       </c>
@@ -4613,12 +4193,12 @@
       <c r="E77" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F77" s="53"/>
-      <c r="G77" s="41"/>
+      <c r="F77" s="36"/>
+      <c r="G77" s="39"/>
     </row>
     <row r="78" spans="1:7" ht="16.5">
-      <c r="A78" s="41"/>
-      <c r="B78" s="50"/>
+      <c r="A78" s="39"/>
+      <c r="B78" s="48"/>
       <c r="C78" s="7" t="s">
         <v>149</v>
       </c>
@@ -4628,12 +4208,12 @@
       <c r="E78" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F78" s="53"/>
-      <c r="G78" s="41"/>
+      <c r="F78" s="36"/>
+      <c r="G78" s="39"/>
     </row>
     <row r="79" spans="1:7" ht="16.5">
-      <c r="A79" s="41"/>
-      <c r="B79" s="50"/>
+      <c r="A79" s="39"/>
+      <c r="B79" s="48"/>
       <c r="C79" s="7" t="s">
         <v>150</v>
       </c>
@@ -4643,12 +4223,12 @@
       <c r="E79" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F79" s="53"/>
-      <c r="G79" s="41"/>
+      <c r="F79" s="36"/>
+      <c r="G79" s="39"/>
     </row>
     <row r="80" spans="1:7" ht="16.5">
-      <c r="A80" s="41"/>
-      <c r="B80" s="50"/>
+      <c r="A80" s="39"/>
+      <c r="B80" s="48"/>
       <c r="C80" s="7" t="s">
         <v>154</v>
       </c>
@@ -4658,12 +4238,12 @@
       <c r="E80" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F80" s="53"/>
-      <c r="G80" s="41"/>
+      <c r="F80" s="36"/>
+      <c r="G80" s="39"/>
     </row>
     <row r="81" spans="1:7" ht="16.5">
-      <c r="A81" s="41"/>
-      <c r="B81" s="50"/>
+      <c r="A81" s="39"/>
+      <c r="B81" s="48"/>
       <c r="C81" s="7" t="s">
         <v>155</v>
       </c>
@@ -4673,12 +4253,12 @@
       <c r="E81" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F81" s="53"/>
-      <c r="G81" s="41"/>
+      <c r="F81" s="36"/>
+      <c r="G81" s="39"/>
     </row>
     <row r="82" spans="1:7" ht="16.5">
-      <c r="A82" s="41"/>
-      <c r="B82" s="50"/>
+      <c r="A82" s="39"/>
+      <c r="B82" s="48"/>
       <c r="C82" s="7" t="s">
         <v>156</v>
       </c>
@@ -4688,14 +4268,14 @@
       <c r="E82" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F82" s="53"/>
-      <c r="G82" s="41"/>
+      <c r="F82" s="36"/>
+      <c r="G82" s="39"/>
     </row>
     <row r="83" spans="1:7" ht="16.5">
-      <c r="A83" s="39">
+      <c r="A83" s="38">
         <v>7</v>
       </c>
-      <c r="B83" s="54" t="s">
+      <c r="B83" s="46" t="s">
         <v>165</v>
       </c>
       <c r="C83" s="4" t="s">
@@ -4707,16 +4287,16 @@
       <c r="E83" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="F83" s="56" t="s">
+      <c r="F83" s="41" t="s">
         <v>166</v>
       </c>
-      <c r="G83" s="39">
+      <c r="G83" s="38">
         <v>0.91</v>
       </c>
     </row>
     <row r="84" spans="1:7" ht="16.5">
-      <c r="A84" s="39"/>
-      <c r="B84" s="54"/>
+      <c r="A84" s="38"/>
+      <c r="B84" s="46"/>
       <c r="C84" s="7" t="s">
         <v>139</v>
       </c>
@@ -4726,12 +4306,12 @@
       <c r="E84" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F84" s="57"/>
-      <c r="G84" s="39"/>
+      <c r="F84" s="42"/>
+      <c r="G84" s="38"/>
     </row>
     <row r="85" spans="1:7" ht="16.5">
-      <c r="A85" s="39"/>
-      <c r="B85" s="54"/>
+      <c r="A85" s="38"/>
+      <c r="B85" s="46"/>
       <c r="C85" s="7" t="s">
         <v>140</v>
       </c>
@@ -4741,12 +4321,12 @@
       <c r="E85" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F85" s="57"/>
-      <c r="G85" s="39"/>
+      <c r="F85" s="42"/>
+      <c r="G85" s="38"/>
     </row>
     <row r="86" spans="1:7" ht="16.5">
-      <c r="A86" s="39"/>
-      <c r="B86" s="54"/>
+      <c r="A86" s="38"/>
+      <c r="B86" s="46"/>
       <c r="C86" s="7" t="s">
         <v>141</v>
       </c>
@@ -4756,12 +4336,12 @@
       <c r="E86" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F86" s="57"/>
-      <c r="G86" s="39"/>
+      <c r="F86" s="42"/>
+      <c r="G86" s="38"/>
     </row>
     <row r="87" spans="1:7" ht="16.5">
-      <c r="A87" s="39"/>
-      <c r="B87" s="54"/>
+      <c r="A87" s="38"/>
+      <c r="B87" s="46"/>
       <c r="C87" s="7" t="s">
         <v>142</v>
       </c>
@@ -4771,12 +4351,12 @@
       <c r="E87" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F87" s="57"/>
-      <c r="G87" s="39"/>
+      <c r="F87" s="42"/>
+      <c r="G87" s="38"/>
     </row>
     <row r="88" spans="1:7" ht="16.5">
-      <c r="A88" s="39"/>
-      <c r="B88" s="54"/>
+      <c r="A88" s="38"/>
+      <c r="B88" s="46"/>
       <c r="C88" s="7" t="s">
         <v>143</v>
       </c>
@@ -4786,12 +4366,12 @@
       <c r="E88" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F88" s="57"/>
-      <c r="G88" s="39"/>
+      <c r="F88" s="42"/>
+      <c r="G88" s="38"/>
     </row>
     <row r="89" spans="1:7" ht="16.5">
-      <c r="A89" s="39"/>
-      <c r="B89" s="54"/>
+      <c r="A89" s="38"/>
+      <c r="B89" s="46"/>
       <c r="C89" s="7" t="s">
         <v>144</v>
       </c>
@@ -4801,12 +4381,12 @@
       <c r="E89" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F89" s="57"/>
-      <c r="G89" s="39"/>
+      <c r="F89" s="42"/>
+      <c r="G89" s="38"/>
     </row>
     <row r="90" spans="1:7" ht="16.5">
-      <c r="A90" s="39"/>
-      <c r="B90" s="54"/>
+      <c r="A90" s="38"/>
+      <c r="B90" s="46"/>
       <c r="C90" s="7" t="s">
         <v>145</v>
       </c>
@@ -4816,12 +4396,12 @@
       <c r="E90" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F90" s="57"/>
-      <c r="G90" s="39"/>
+      <c r="F90" s="42"/>
+      <c r="G90" s="38"/>
     </row>
     <row r="91" spans="1:7" ht="16.5">
-      <c r="A91" s="39"/>
-      <c r="B91" s="54"/>
+      <c r="A91" s="38"/>
+      <c r="B91" s="46"/>
       <c r="C91" s="7" t="s">
         <v>149</v>
       </c>
@@ -4831,12 +4411,12 @@
       <c r="E91" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F91" s="57"/>
-      <c r="G91" s="39"/>
+      <c r="F91" s="42"/>
+      <c r="G91" s="38"/>
     </row>
     <row r="92" spans="1:7" ht="16.5">
-      <c r="A92" s="39"/>
-      <c r="B92" s="54"/>
+      <c r="A92" s="38"/>
+      <c r="B92" s="46"/>
       <c r="C92" s="7" t="s">
         <v>150</v>
       </c>
@@ -4846,12 +4426,12 @@
       <c r="E92" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F92" s="57"/>
-      <c r="G92" s="39"/>
+      <c r="F92" s="42"/>
+      <c r="G92" s="38"/>
     </row>
     <row r="93" spans="1:7" ht="16.5">
-      <c r="A93" s="39"/>
-      <c r="B93" s="54"/>
+      <c r="A93" s="38"/>
+      <c r="B93" s="46"/>
       <c r="C93" s="7" t="s">
         <v>154</v>
       </c>
@@ -4861,12 +4441,12 @@
       <c r="E93" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F93" s="57"/>
-      <c r="G93" s="39"/>
+      <c r="F93" s="42"/>
+      <c r="G93" s="38"/>
     </row>
     <row r="94" spans="1:7" ht="16.5">
-      <c r="A94" s="39"/>
-      <c r="B94" s="54"/>
+      <c r="A94" s="38"/>
+      <c r="B94" s="46"/>
       <c r="C94" s="7" t="s">
         <v>155</v>
       </c>
@@ -4876,12 +4456,12 @@
       <c r="E94" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F94" s="57"/>
-      <c r="G94" s="39"/>
+      <c r="F94" s="42"/>
+      <c r="G94" s="38"/>
     </row>
     <row r="95" spans="1:7" ht="16.5">
-      <c r="A95" s="39"/>
-      <c r="B95" s="54"/>
+      <c r="A95" s="38"/>
+      <c r="B95" s="46"/>
       <c r="C95" s="9" t="s">
         <v>156</v>
       </c>
@@ -4891,14 +4471,14 @@
       <c r="E95" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="F95" s="57"/>
-      <c r="G95" s="39"/>
+      <c r="F95" s="42"/>
+      <c r="G95" s="38"/>
     </row>
     <row r="96" spans="1:7" ht="16.5">
-      <c r="A96" s="41">
+      <c r="A96" s="39">
         <v>8</v>
       </c>
-      <c r="B96" s="50" t="s">
+      <c r="B96" s="48" t="s">
         <v>167</v>
       </c>
       <c r="C96" s="7" t="s">
@@ -4910,16 +4490,16 @@
       <c r="E96" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F96" s="58" t="s">
+      <c r="F96" s="35" t="s">
         <v>168</v>
       </c>
-      <c r="G96" s="41">
+      <c r="G96" s="39">
         <v>1.01</v>
       </c>
     </row>
     <row r="97" spans="1:7" ht="16.5">
-      <c r="A97" s="41"/>
-      <c r="B97" s="50"/>
+      <c r="A97" s="39"/>
+      <c r="B97" s="48"/>
       <c r="C97" s="7" t="s">
         <v>139</v>
       </c>
@@ -4929,12 +4509,12 @@
       <c r="E97" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F97" s="53"/>
-      <c r="G97" s="41"/>
+      <c r="F97" s="36"/>
+      <c r="G97" s="39"/>
     </row>
     <row r="98" spans="1:7" ht="16.5">
-      <c r="A98" s="41"/>
-      <c r="B98" s="50"/>
+      <c r="A98" s="39"/>
+      <c r="B98" s="48"/>
       <c r="C98" s="7" t="s">
         <v>140</v>
       </c>
@@ -4944,12 +4524,12 @@
       <c r="E98" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F98" s="53"/>
-      <c r="G98" s="41"/>
+      <c r="F98" s="36"/>
+      <c r="G98" s="39"/>
     </row>
     <row r="99" spans="1:7" ht="16.5">
-      <c r="A99" s="41"/>
-      <c r="B99" s="50"/>
+      <c r="A99" s="39"/>
+      <c r="B99" s="48"/>
       <c r="C99" s="7" t="s">
         <v>141</v>
       </c>
@@ -4959,12 +4539,12 @@
       <c r="E99" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F99" s="53"/>
-      <c r="G99" s="41"/>
+      <c r="F99" s="36"/>
+      <c r="G99" s="39"/>
     </row>
     <row r="100" spans="1:7" ht="16.5">
-      <c r="A100" s="41"/>
-      <c r="B100" s="50"/>
+      <c r="A100" s="39"/>
+      <c r="B100" s="48"/>
       <c r="C100" s="7" t="s">
         <v>142</v>
       </c>
@@ -4974,12 +4554,12 @@
       <c r="E100" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F100" s="53"/>
-      <c r="G100" s="41"/>
+      <c r="F100" s="36"/>
+      <c r="G100" s="39"/>
     </row>
     <row r="101" spans="1:7" ht="16.5">
-      <c r="A101" s="41"/>
-      <c r="B101" s="50"/>
+      <c r="A101" s="39"/>
+      <c r="B101" s="48"/>
       <c r="C101" s="7" t="s">
         <v>143</v>
       </c>
@@ -4989,12 +4569,12 @@
       <c r="E101" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F101" s="53"/>
-      <c r="G101" s="41"/>
+      <c r="F101" s="36"/>
+      <c r="G101" s="39"/>
     </row>
     <row r="102" spans="1:7" ht="16.5">
-      <c r="A102" s="41"/>
-      <c r="B102" s="50"/>
+      <c r="A102" s="39"/>
+      <c r="B102" s="48"/>
       <c r="C102" s="7" t="s">
         <v>144</v>
       </c>
@@ -5004,12 +4584,12 @@
       <c r="E102" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F102" s="53"/>
-      <c r="G102" s="41"/>
+      <c r="F102" s="36"/>
+      <c r="G102" s="39"/>
     </row>
     <row r="103" spans="1:7" ht="16.5">
-      <c r="A103" s="41"/>
-      <c r="B103" s="50"/>
+      <c r="A103" s="39"/>
+      <c r="B103" s="48"/>
       <c r="C103" s="7" t="s">
         <v>145</v>
       </c>
@@ -5019,12 +4599,12 @@
       <c r="E103" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F103" s="53"/>
-      <c r="G103" s="41"/>
+      <c r="F103" s="36"/>
+      <c r="G103" s="39"/>
     </row>
     <row r="104" spans="1:7" ht="16.5">
-      <c r="A104" s="41"/>
-      <c r="B104" s="50"/>
+      <c r="A104" s="39"/>
+      <c r="B104" s="48"/>
       <c r="C104" s="7" t="s">
         <v>149</v>
       </c>
@@ -5034,12 +4614,12 @@
       <c r="E104" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F104" s="53"/>
-      <c r="G104" s="41"/>
+      <c r="F104" s="36"/>
+      <c r="G104" s="39"/>
     </row>
     <row r="105" spans="1:7" ht="16.5">
-      <c r="A105" s="41"/>
-      <c r="B105" s="50"/>
+      <c r="A105" s="39"/>
+      <c r="B105" s="48"/>
       <c r="C105" s="7" t="s">
         <v>150</v>
       </c>
@@ -5049,12 +4629,12 @@
       <c r="E105" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F105" s="53"/>
-      <c r="G105" s="41"/>
+      <c r="F105" s="36"/>
+      <c r="G105" s="39"/>
     </row>
     <row r="106" spans="1:7" ht="16.5">
-      <c r="A106" s="41"/>
-      <c r="B106" s="50"/>
+      <c r="A106" s="39"/>
+      <c r="B106" s="48"/>
       <c r="C106" s="7" t="s">
         <v>154</v>
       </c>
@@ -5064,12 +4644,12 @@
       <c r="E106" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F106" s="53"/>
-      <c r="G106" s="41"/>
+      <c r="F106" s="36"/>
+      <c r="G106" s="39"/>
     </row>
     <row r="107" spans="1:7" ht="16.5">
-      <c r="A107" s="41"/>
-      <c r="B107" s="50"/>
+      <c r="A107" s="39"/>
+      <c r="B107" s="48"/>
       <c r="C107" s="7" t="s">
         <v>155</v>
       </c>
@@ -5079,12 +4659,12 @@
       <c r="E107" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F107" s="53"/>
-      <c r="G107" s="41"/>
+      <c r="F107" s="36"/>
+      <c r="G107" s="39"/>
     </row>
     <row r="108" spans="1:7" ht="16.5">
-      <c r="A108" s="42"/>
-      <c r="B108" s="51"/>
+      <c r="A108" s="40"/>
+      <c r="B108" s="49"/>
       <c r="C108" s="7" t="s">
         <v>156</v>
       </c>
@@ -5094,14 +4674,14 @@
       <c r="E108" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F108" s="59"/>
-      <c r="G108" s="42"/>
+      <c r="F108" s="37"/>
+      <c r="G108" s="40"/>
     </row>
     <row r="109" spans="1:7" ht="16.5">
-      <c r="A109" s="61">
-        <v>9</v>
-      </c>
-      <c r="B109" s="50" t="s">
+      <c r="A109" s="44">
+        <v>9</v>
+      </c>
+      <c r="B109" s="48" t="s">
         <v>169</v>
       </c>
       <c r="C109" s="12" t="s">
@@ -5113,16 +4693,16 @@
       <c r="E109" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="F109" s="58" t="s">
+      <c r="F109" s="35" t="s">
         <v>170</v>
       </c>
-      <c r="G109" s="41">
+      <c r="G109" s="39">
         <v>0.93</v>
       </c>
     </row>
     <row r="110" spans="1:7" ht="16.5">
-      <c r="A110" s="61"/>
-      <c r="B110" s="50"/>
+      <c r="A110" s="44"/>
+      <c r="B110" s="48"/>
       <c r="C110" s="12" t="s">
         <v>139</v>
       </c>
@@ -5132,12 +4712,12 @@
       <c r="E110" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="F110" s="58"/>
-      <c r="G110" s="41"/>
+      <c r="F110" s="35"/>
+      <c r="G110" s="39"/>
     </row>
     <row r="111" spans="1:7" ht="16.5">
-      <c r="A111" s="61"/>
-      <c r="B111" s="50"/>
+      <c r="A111" s="44"/>
+      <c r="B111" s="48"/>
       <c r="C111" s="12" t="s">
         <v>140</v>
       </c>
@@ -5147,12 +4727,12 @@
       <c r="E111" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="F111" s="58"/>
-      <c r="G111" s="41"/>
+      <c r="F111" s="35"/>
+      <c r="G111" s="39"/>
     </row>
     <row r="112" spans="1:7" ht="16.5">
-      <c r="A112" s="61"/>
-      <c r="B112" s="50"/>
+      <c r="A112" s="44"/>
+      <c r="B112" s="48"/>
       <c r="C112" s="12" t="s">
         <v>141</v>
       </c>
@@ -5162,12 +4742,12 @@
       <c r="E112" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="F112" s="58"/>
-      <c r="G112" s="41"/>
+      <c r="F112" s="35"/>
+      <c r="G112" s="39"/>
     </row>
     <row r="113" spans="1:7" ht="16.5">
-      <c r="A113" s="61"/>
-      <c r="B113" s="50"/>
+      <c r="A113" s="44"/>
+      <c r="B113" s="48"/>
       <c r="C113" s="12" t="s">
         <v>142</v>
       </c>
@@ -5177,12 +4757,12 @@
       <c r="E113" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="F113" s="58"/>
-      <c r="G113" s="41"/>
+      <c r="F113" s="35"/>
+      <c r="G113" s="39"/>
     </row>
     <row r="114" spans="1:7" ht="16.5">
-      <c r="A114" s="61"/>
-      <c r="B114" s="50"/>
+      <c r="A114" s="44"/>
+      <c r="B114" s="48"/>
       <c r="C114" s="12" t="s">
         <v>143</v>
       </c>
@@ -5192,12 +4772,12 @@
       <c r="E114" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="F114" s="58"/>
-      <c r="G114" s="41"/>
+      <c r="F114" s="35"/>
+      <c r="G114" s="39"/>
     </row>
     <row r="115" spans="1:7" ht="16.5">
-      <c r="A115" s="61"/>
-      <c r="B115" s="50"/>
+      <c r="A115" s="44"/>
+      <c r="B115" s="48"/>
       <c r="C115" s="12" t="s">
         <v>144</v>
       </c>
@@ -5207,12 +4787,12 @@
       <c r="E115" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="F115" s="58"/>
-      <c r="G115" s="41"/>
+      <c r="F115" s="35"/>
+      <c r="G115" s="39"/>
     </row>
     <row r="116" spans="1:7" ht="16.5">
-      <c r="A116" s="61"/>
-      <c r="B116" s="50"/>
+      <c r="A116" s="44"/>
+      <c r="B116" s="48"/>
       <c r="C116" s="12" t="s">
         <v>145</v>
       </c>
@@ -5222,12 +4802,12 @@
       <c r="E116" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="F116" s="58"/>
-      <c r="G116" s="41"/>
+      <c r="F116" s="35"/>
+      <c r="G116" s="39"/>
     </row>
     <row r="117" spans="1:7" ht="16.5">
-      <c r="A117" s="61"/>
-      <c r="B117" s="50"/>
+      <c r="A117" s="44"/>
+      <c r="B117" s="48"/>
       <c r="C117" s="12" t="s">
         <v>149</v>
       </c>
@@ -5237,12 +4817,12 @@
       <c r="E117" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="F117" s="58"/>
-      <c r="G117" s="41"/>
+      <c r="F117" s="35"/>
+      <c r="G117" s="39"/>
     </row>
     <row r="118" spans="1:7" ht="16.5">
-      <c r="A118" s="61"/>
-      <c r="B118" s="50"/>
+      <c r="A118" s="44"/>
+      <c r="B118" s="48"/>
       <c r="C118" s="12" t="s">
         <v>150</v>
       </c>
@@ -5252,12 +4832,12 @@
       <c r="E118" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="F118" s="58"/>
-      <c r="G118" s="41"/>
+      <c r="F118" s="35"/>
+      <c r="G118" s="39"/>
     </row>
     <row r="119" spans="1:7" ht="16.5">
-      <c r="A119" s="61"/>
-      <c r="B119" s="50"/>
+      <c r="A119" s="44"/>
+      <c r="B119" s="48"/>
       <c r="C119" s="12" t="s">
         <v>154</v>
       </c>
@@ -5267,12 +4847,12 @@
       <c r="E119" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="F119" s="58"/>
-      <c r="G119" s="41"/>
+      <c r="F119" s="35"/>
+      <c r="G119" s="39"/>
     </row>
     <row r="120" spans="1:7" ht="16.5">
-      <c r="A120" s="61"/>
-      <c r="B120" s="50"/>
+      <c r="A120" s="44"/>
+      <c r="B120" s="48"/>
       <c r="C120" s="12" t="s">
         <v>155</v>
       </c>
@@ -5282,12 +4862,12 @@
       <c r="E120" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="F120" s="58"/>
-      <c r="G120" s="41"/>
+      <c r="F120" s="35"/>
+      <c r="G120" s="39"/>
     </row>
     <row r="121" spans="1:7" ht="16.5">
-      <c r="A121" s="62"/>
-      <c r="B121" s="51"/>
+      <c r="A121" s="45"/>
+      <c r="B121" s="49"/>
       <c r="C121" s="14" t="s">
         <v>156</v>
       </c>
@@ -5297,14 +4877,14 @@
       <c r="E121" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="F121" s="60"/>
-      <c r="G121" s="42"/>
+      <c r="F121" s="43"/>
+      <c r="G121" s="40"/>
     </row>
     <row r="122" spans="1:7" ht="16.5">
-      <c r="A122" s="41">
+      <c r="A122" s="39">
         <v>10</v>
       </c>
-      <c r="B122" s="50" t="s">
+      <c r="B122" s="48" t="s">
         <v>171</v>
       </c>
       <c r="C122" s="7" t="s">
@@ -5316,16 +4896,16 @@
       <c r="E122" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F122" s="58" t="s">
+      <c r="F122" s="35" t="s">
         <v>172</v>
       </c>
-      <c r="G122" s="41">
+      <c r="G122" s="39">
         <v>1.76</v>
       </c>
     </row>
     <row r="123" spans="1:7" ht="16.5">
-      <c r="A123" s="41"/>
-      <c r="B123" s="50"/>
+      <c r="A123" s="39"/>
+      <c r="B123" s="48"/>
       <c r="C123" s="7" t="s">
         <v>139</v>
       </c>
@@ -5335,12 +4915,12 @@
       <c r="E123" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F123" s="53"/>
-      <c r="G123" s="41"/>
+      <c r="F123" s="36"/>
+      <c r="G123" s="39"/>
     </row>
     <row r="124" spans="1:7" ht="16.5">
-      <c r="A124" s="41"/>
-      <c r="B124" s="50"/>
+      <c r="A124" s="39"/>
+      <c r="B124" s="48"/>
       <c r="C124" s="7" t="s">
         <v>140</v>
       </c>
@@ -5350,12 +4930,12 @@
       <c r="E124" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F124" s="53"/>
-      <c r="G124" s="41"/>
+      <c r="F124" s="36"/>
+      <c r="G124" s="39"/>
     </row>
     <row r="125" spans="1:7" ht="16.5">
-      <c r="A125" s="41"/>
-      <c r="B125" s="50"/>
+      <c r="A125" s="39"/>
+      <c r="B125" s="48"/>
       <c r="C125" s="7" t="s">
         <v>141</v>
       </c>
@@ -5365,12 +4945,12 @@
       <c r="E125" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F125" s="53"/>
-      <c r="G125" s="41"/>
+      <c r="F125" s="36"/>
+      <c r="G125" s="39"/>
     </row>
     <row r="126" spans="1:7" ht="16.5">
-      <c r="A126" s="41"/>
-      <c r="B126" s="50"/>
+      <c r="A126" s="39"/>
+      <c r="B126" s="48"/>
       <c r="C126" s="7" t="s">
         <v>142</v>
       </c>
@@ -5380,12 +4960,12 @@
       <c r="E126" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F126" s="53"/>
-      <c r="G126" s="41"/>
+      <c r="F126" s="36"/>
+      <c r="G126" s="39"/>
     </row>
     <row r="127" spans="1:7" ht="16.5">
-      <c r="A127" s="41"/>
-      <c r="B127" s="50"/>
+      <c r="A127" s="39"/>
+      <c r="B127" s="48"/>
       <c r="C127" s="7" t="s">
         <v>143</v>
       </c>
@@ -5395,12 +4975,12 @@
       <c r="E127" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F127" s="53"/>
-      <c r="G127" s="41"/>
+      <c r="F127" s="36"/>
+      <c r="G127" s="39"/>
     </row>
     <row r="128" spans="1:7" ht="16.5">
-      <c r="A128" s="41"/>
-      <c r="B128" s="50"/>
+      <c r="A128" s="39"/>
+      <c r="B128" s="48"/>
       <c r="C128" s="7" t="s">
         <v>144</v>
       </c>
@@ -5410,12 +4990,12 @@
       <c r="E128" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F128" s="53"/>
-      <c r="G128" s="41"/>
+      <c r="F128" s="36"/>
+      <c r="G128" s="39"/>
     </row>
     <row r="129" spans="1:7" ht="16.5">
-      <c r="A129" s="41"/>
-      <c r="B129" s="50"/>
+      <c r="A129" s="39"/>
+      <c r="B129" s="48"/>
       <c r="C129" s="7" t="s">
         <v>145</v>
       </c>
@@ -5425,12 +5005,12 @@
       <c r="E129" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F129" s="53"/>
-      <c r="G129" s="41"/>
+      <c r="F129" s="36"/>
+      <c r="G129" s="39"/>
     </row>
     <row r="130" spans="1:7" ht="16.5">
-      <c r="A130" s="41"/>
-      <c r="B130" s="50"/>
+      <c r="A130" s="39"/>
+      <c r="B130" s="48"/>
       <c r="C130" s="7" t="s">
         <v>149</v>
       </c>
@@ -5440,12 +5020,12 @@
       <c r="E130" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F130" s="53"/>
-      <c r="G130" s="41"/>
+      <c r="F130" s="36"/>
+      <c r="G130" s="39"/>
     </row>
     <row r="131" spans="1:7" ht="16.5">
-      <c r="A131" s="41"/>
-      <c r="B131" s="50"/>
+      <c r="A131" s="39"/>
+      <c r="B131" s="48"/>
       <c r="C131" s="7" t="s">
         <v>150</v>
       </c>
@@ -5455,12 +5035,12 @@
       <c r="E131" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F131" s="53"/>
-      <c r="G131" s="41"/>
+      <c r="F131" s="36"/>
+      <c r="G131" s="39"/>
     </row>
     <row r="132" spans="1:7" ht="16.5">
-      <c r="A132" s="41"/>
-      <c r="B132" s="50"/>
+      <c r="A132" s="39"/>
+      <c r="B132" s="48"/>
       <c r="C132" s="7" t="s">
         <v>154</v>
       </c>
@@ -5470,12 +5050,12 @@
       <c r="E132" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F132" s="53"/>
-      <c r="G132" s="41"/>
+      <c r="F132" s="36"/>
+      <c r="G132" s="39"/>
     </row>
     <row r="133" spans="1:7" ht="16.5">
-      <c r="A133" s="41"/>
-      <c r="B133" s="50"/>
+      <c r="A133" s="39"/>
+      <c r="B133" s="48"/>
       <c r="C133" s="7" t="s">
         <v>155</v>
       </c>
@@ -5485,12 +5065,12 @@
       <c r="E133" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F133" s="53"/>
-      <c r="G133" s="41"/>
+      <c r="F133" s="36"/>
+      <c r="G133" s="39"/>
     </row>
     <row r="134" spans="1:7" ht="16.5">
-      <c r="A134" s="42"/>
-      <c r="B134" s="51"/>
+      <c r="A134" s="40"/>
+      <c r="B134" s="49"/>
       <c r="C134" s="9" t="s">
         <v>156</v>
       </c>
@@ -5500,14 +5080,14 @@
       <c r="E134" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="F134" s="59"/>
-      <c r="G134" s="42"/>
+      <c r="F134" s="37"/>
+      <c r="G134" s="40"/>
     </row>
     <row r="135" spans="1:7" ht="16.5">
-      <c r="A135" s="41">
-        <v>11</v>
-      </c>
-      <c r="B135" s="50" t="s">
+      <c r="A135" s="39">
+        <v>11</v>
+      </c>
+      <c r="B135" s="48" t="s">
         <v>173</v>
       </c>
       <c r="C135" s="7" t="s">
@@ -5519,16 +5099,16 @@
       <c r="E135" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F135" s="58" t="s">
+      <c r="F135" s="35" t="s">
         <v>174</v>
       </c>
-      <c r="G135" s="41">
+      <c r="G135" s="39">
         <v>1.19</v>
       </c>
     </row>
     <row r="136" spans="1:7" ht="16.5">
-      <c r="A136" s="41"/>
-      <c r="B136" s="50"/>
+      <c r="A136" s="39"/>
+      <c r="B136" s="48"/>
       <c r="C136" s="7" t="s">
         <v>139</v>
       </c>
@@ -5538,12 +5118,12 @@
       <c r="E136" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F136" s="53"/>
-      <c r="G136" s="41"/>
+      <c r="F136" s="36"/>
+      <c r="G136" s="39"/>
     </row>
     <row r="137" spans="1:7" ht="16.5">
-      <c r="A137" s="41"/>
-      <c r="B137" s="50"/>
+      <c r="A137" s="39"/>
+      <c r="B137" s="48"/>
       <c r="C137" s="7" t="s">
         <v>140</v>
       </c>
@@ -5553,12 +5133,12 @@
       <c r="E137" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F137" s="53"/>
-      <c r="G137" s="41"/>
+      <c r="F137" s="36"/>
+      <c r="G137" s="39"/>
     </row>
     <row r="138" spans="1:7" ht="16.5">
-      <c r="A138" s="41"/>
-      <c r="B138" s="50"/>
+      <c r="A138" s="39"/>
+      <c r="B138" s="48"/>
       <c r="C138" s="7" t="s">
         <v>141</v>
       </c>
@@ -5568,12 +5148,12 @@
       <c r="E138" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F138" s="53"/>
-      <c r="G138" s="41"/>
+      <c r="F138" s="36"/>
+      <c r="G138" s="39"/>
     </row>
     <row r="139" spans="1:7" ht="16.5">
-      <c r="A139" s="41"/>
-      <c r="B139" s="50"/>
+      <c r="A139" s="39"/>
+      <c r="B139" s="48"/>
       <c r="C139" s="7" t="s">
         <v>142</v>
       </c>
@@ -5583,12 +5163,12 @@
       <c r="E139" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F139" s="53"/>
-      <c r="G139" s="41"/>
+      <c r="F139" s="36"/>
+      <c r="G139" s="39"/>
     </row>
     <row r="140" spans="1:7" ht="16.5">
-      <c r="A140" s="41"/>
-      <c r="B140" s="50"/>
+      <c r="A140" s="39"/>
+      <c r="B140" s="48"/>
       <c r="C140" s="7" t="s">
         <v>143</v>
       </c>
@@ -5598,12 +5178,12 @@
       <c r="E140" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F140" s="53"/>
-      <c r="G140" s="41"/>
+      <c r="F140" s="36"/>
+      <c r="G140" s="39"/>
     </row>
     <row r="141" spans="1:7" ht="16.5">
-      <c r="A141" s="41"/>
-      <c r="B141" s="50"/>
+      <c r="A141" s="39"/>
+      <c r="B141" s="48"/>
       <c r="C141" s="7" t="s">
         <v>144</v>
       </c>
@@ -5613,12 +5193,12 @@
       <c r="E141" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F141" s="53"/>
-      <c r="G141" s="41"/>
+      <c r="F141" s="36"/>
+      <c r="G141" s="39"/>
     </row>
     <row r="142" spans="1:7" ht="16.5">
-      <c r="A142" s="41"/>
-      <c r="B142" s="50"/>
+      <c r="A142" s="39"/>
+      <c r="B142" s="48"/>
       <c r="C142" s="7" t="s">
         <v>145</v>
       </c>
@@ -5628,12 +5208,12 @@
       <c r="E142" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F142" s="53"/>
-      <c r="G142" s="41"/>
+      <c r="F142" s="36"/>
+      <c r="G142" s="39"/>
     </row>
     <row r="143" spans="1:7" ht="16.5">
-      <c r="A143" s="41"/>
-      <c r="B143" s="50"/>
+      <c r="A143" s="39"/>
+      <c r="B143" s="48"/>
       <c r="C143" s="7" t="s">
         <v>149</v>
       </c>
@@ -5643,12 +5223,12 @@
       <c r="E143" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F143" s="53"/>
-      <c r="G143" s="41"/>
+      <c r="F143" s="36"/>
+      <c r="G143" s="39"/>
     </row>
     <row r="144" spans="1:7" ht="16.5">
-      <c r="A144" s="41"/>
-      <c r="B144" s="50"/>
+      <c r="A144" s="39"/>
+      <c r="B144" s="48"/>
       <c r="C144" s="7" t="s">
         <v>150</v>
       </c>
@@ -5658,12 +5238,12 @@
       <c r="E144" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F144" s="53"/>
-      <c r="G144" s="41"/>
+      <c r="F144" s="36"/>
+      <c r="G144" s="39"/>
     </row>
     <row r="145" spans="1:7" ht="16.5">
-      <c r="A145" s="41"/>
-      <c r="B145" s="50"/>
+      <c r="A145" s="39"/>
+      <c r="B145" s="48"/>
       <c r="C145" s="7" t="s">
         <v>154</v>
       </c>
@@ -5673,12 +5253,12 @@
       <c r="E145" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F145" s="53"/>
-      <c r="G145" s="41"/>
+      <c r="F145" s="36"/>
+      <c r="G145" s="39"/>
     </row>
     <row r="146" spans="1:7" ht="16.5">
-      <c r="A146" s="41"/>
-      <c r="B146" s="50"/>
+      <c r="A146" s="39"/>
+      <c r="B146" s="48"/>
       <c r="C146" s="7" t="s">
         <v>155</v>
       </c>
@@ -5688,12 +5268,12 @@
       <c r="E146" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F146" s="53"/>
-      <c r="G146" s="41"/>
+      <c r="F146" s="36"/>
+      <c r="G146" s="39"/>
     </row>
     <row r="147" spans="1:7" ht="16.5">
-      <c r="A147" s="42"/>
-      <c r="B147" s="51"/>
+      <c r="A147" s="40"/>
+      <c r="B147" s="49"/>
       <c r="C147" s="9" t="s">
         <v>156</v>
       </c>
@@ -5703,14 +5283,14 @@
       <c r="E147" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="F147" s="59"/>
-      <c r="G147" s="42"/>
+      <c r="F147" s="37"/>
+      <c r="G147" s="40"/>
     </row>
     <row r="148" spans="1:7" ht="16.5">
-      <c r="A148" s="41">
+      <c r="A148" s="39">
         <v>12</v>
       </c>
-      <c r="B148" s="50" t="s">
+      <c r="B148" s="48" t="s">
         <v>175</v>
       </c>
       <c r="C148" s="7" t="s">
@@ -5722,16 +5302,16 @@
       <c r="E148" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F148" s="58" t="s">
+      <c r="F148" s="35" t="s">
         <v>77</v>
       </c>
-      <c r="G148" s="41">
+      <c r="G148" s="39">
         <v>1.08</v>
       </c>
     </row>
     <row r="149" spans="1:7" ht="16.5">
-      <c r="A149" s="41"/>
-      <c r="B149" s="50"/>
+      <c r="A149" s="39"/>
+      <c r="B149" s="48"/>
       <c r="C149" s="7" t="s">
         <v>139</v>
       </c>
@@ -5741,12 +5321,12 @@
       <c r="E149" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F149" s="53"/>
-      <c r="G149" s="41"/>
+      <c r="F149" s="36"/>
+      <c r="G149" s="39"/>
     </row>
     <row r="150" spans="1:7" ht="16.5">
-      <c r="A150" s="41"/>
-      <c r="B150" s="50"/>
+      <c r="A150" s="39"/>
+      <c r="B150" s="48"/>
       <c r="C150" s="7" t="s">
         <v>140</v>
       </c>
@@ -5756,12 +5336,12 @@
       <c r="E150" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F150" s="53"/>
-      <c r="G150" s="41"/>
+      <c r="F150" s="36"/>
+      <c r="G150" s="39"/>
     </row>
     <row r="151" spans="1:7" ht="16.5">
-      <c r="A151" s="41"/>
-      <c r="B151" s="50"/>
+      <c r="A151" s="39"/>
+      <c r="B151" s="48"/>
       <c r="C151" s="7" t="s">
         <v>141</v>
       </c>
@@ -5771,12 +5351,12 @@
       <c r="E151" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F151" s="53"/>
-      <c r="G151" s="41"/>
+      <c r="F151" s="36"/>
+      <c r="G151" s="39"/>
     </row>
     <row r="152" spans="1:7" ht="16.5">
-      <c r="A152" s="41"/>
-      <c r="B152" s="50"/>
+      <c r="A152" s="39"/>
+      <c r="B152" s="48"/>
       <c r="C152" s="7" t="s">
         <v>142</v>
       </c>
@@ -5786,12 +5366,12 @@
       <c r="E152" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F152" s="53"/>
-      <c r="G152" s="41"/>
+      <c r="F152" s="36"/>
+      <c r="G152" s="39"/>
     </row>
     <row r="153" spans="1:7" ht="16.5">
-      <c r="A153" s="41"/>
-      <c r="B153" s="50"/>
+      <c r="A153" s="39"/>
+      <c r="B153" s="48"/>
       <c r="C153" s="7" t="s">
         <v>143</v>
       </c>
@@ -5801,12 +5381,12 @@
       <c r="E153" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F153" s="53"/>
-      <c r="G153" s="41"/>
+      <c r="F153" s="36"/>
+      <c r="G153" s="39"/>
     </row>
     <row r="154" spans="1:7" ht="16.5">
-      <c r="A154" s="41"/>
-      <c r="B154" s="50"/>
+      <c r="A154" s="39"/>
+      <c r="B154" s="48"/>
       <c r="C154" s="7" t="s">
         <v>144</v>
       </c>
@@ -5816,12 +5396,12 @@
       <c r="E154" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F154" s="53"/>
-      <c r="G154" s="41"/>
+      <c r="F154" s="36"/>
+      <c r="G154" s="39"/>
     </row>
     <row r="155" spans="1:7" ht="16.5">
-      <c r="A155" s="41"/>
-      <c r="B155" s="50"/>
+      <c r="A155" s="39"/>
+      <c r="B155" s="48"/>
       <c r="C155" s="7" t="s">
         <v>145</v>
       </c>
@@ -5831,12 +5411,12 @@
       <c r="E155" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F155" s="53"/>
-      <c r="G155" s="41"/>
+      <c r="F155" s="36"/>
+      <c r="G155" s="39"/>
     </row>
     <row r="156" spans="1:7" ht="16.5">
-      <c r="A156" s="41"/>
-      <c r="B156" s="50"/>
+      <c r="A156" s="39"/>
+      <c r="B156" s="48"/>
       <c r="C156" s="7" t="s">
         <v>149</v>
       </c>
@@ -5846,12 +5426,12 @@
       <c r="E156" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F156" s="53"/>
-      <c r="G156" s="41"/>
+      <c r="F156" s="36"/>
+      <c r="G156" s="39"/>
     </row>
     <row r="157" spans="1:7" ht="16.5">
-      <c r="A157" s="41"/>
-      <c r="B157" s="50"/>
+      <c r="A157" s="39"/>
+      <c r="B157" s="48"/>
       <c r="C157" s="7" t="s">
         <v>150</v>
       </c>
@@ -5861,12 +5441,12 @@
       <c r="E157" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F157" s="53"/>
-      <c r="G157" s="41"/>
+      <c r="F157" s="36"/>
+      <c r="G157" s="39"/>
     </row>
     <row r="158" spans="1:7" ht="16.5">
-      <c r="A158" s="41"/>
-      <c r="B158" s="50"/>
+      <c r="A158" s="39"/>
+      <c r="B158" s="48"/>
       <c r="C158" s="7" t="s">
         <v>154</v>
       </c>
@@ -5876,12 +5456,12 @@
       <c r="E158" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F158" s="53"/>
-      <c r="G158" s="41"/>
+      <c r="F158" s="36"/>
+      <c r="G158" s="39"/>
     </row>
     <row r="159" spans="1:7" ht="16.5">
-      <c r="A159" s="41"/>
-      <c r="B159" s="50"/>
+      <c r="A159" s="39"/>
+      <c r="B159" s="48"/>
       <c r="C159" s="7" t="s">
         <v>155</v>
       </c>
@@ -5891,12 +5471,12 @@
       <c r="E159" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F159" s="53"/>
-      <c r="G159" s="41"/>
+      <c r="F159" s="36"/>
+      <c r="G159" s="39"/>
     </row>
     <row r="160" spans="1:7" ht="16.5">
-      <c r="A160" s="41"/>
-      <c r="B160" s="50"/>
+      <c r="A160" s="39"/>
+      <c r="B160" s="48"/>
       <c r="C160" s="7" t="s">
         <v>156</v>
       </c>
@@ -5906,11 +5486,44 @@
       <c r="E160" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F160" s="53"/>
-      <c r="G160" s="41"/>
+      <c r="F160" s="36"/>
+      <c r="G160" s="39"/>
     </row>
   </sheetData>
   <mergeCells count="49">
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A3:A17"/>
+    <mergeCell ref="A18:A30"/>
+    <mergeCell ref="A31:A43"/>
+    <mergeCell ref="A44:A56"/>
+    <mergeCell ref="F3:F17"/>
+    <mergeCell ref="F18:F30"/>
+    <mergeCell ref="F31:F43"/>
+    <mergeCell ref="F44:F56"/>
+    <mergeCell ref="A135:A147"/>
+    <mergeCell ref="A148:A160"/>
+    <mergeCell ref="B3:B17"/>
+    <mergeCell ref="B18:B30"/>
+    <mergeCell ref="B31:B43"/>
+    <mergeCell ref="B44:B56"/>
+    <mergeCell ref="B57:B69"/>
+    <mergeCell ref="B70:B82"/>
+    <mergeCell ref="B83:B95"/>
+    <mergeCell ref="B96:B108"/>
+    <mergeCell ref="B109:B121"/>
+    <mergeCell ref="B122:B134"/>
+    <mergeCell ref="B135:B147"/>
+    <mergeCell ref="B148:B160"/>
+    <mergeCell ref="A57:A69"/>
+    <mergeCell ref="A70:A82"/>
+    <mergeCell ref="F83:F95"/>
+    <mergeCell ref="F96:F108"/>
+    <mergeCell ref="F109:F121"/>
+    <mergeCell ref="A122:A134"/>
+    <mergeCell ref="A83:A95"/>
+    <mergeCell ref="A96:A108"/>
+    <mergeCell ref="A109:A121"/>
+    <mergeCell ref="F122:F134"/>
     <mergeCell ref="F135:F147"/>
     <mergeCell ref="F148:F160"/>
     <mergeCell ref="G3:G17"/>
@@ -5927,39 +5540,6 @@
     <mergeCell ref="G148:G160"/>
     <mergeCell ref="F57:F69"/>
     <mergeCell ref="F70:F82"/>
-    <mergeCell ref="F83:F95"/>
-    <mergeCell ref="F96:F108"/>
-    <mergeCell ref="F109:F121"/>
-    <mergeCell ref="A122:A134"/>
-    <mergeCell ref="A83:A95"/>
-    <mergeCell ref="A96:A108"/>
-    <mergeCell ref="A109:A121"/>
-    <mergeCell ref="F122:F134"/>
-    <mergeCell ref="A135:A147"/>
-    <mergeCell ref="A148:A160"/>
-    <mergeCell ref="B3:B17"/>
-    <mergeCell ref="B18:B30"/>
-    <mergeCell ref="B31:B43"/>
-    <mergeCell ref="B44:B56"/>
-    <mergeCell ref="B57:B69"/>
-    <mergeCell ref="B70:B82"/>
-    <mergeCell ref="B83:B95"/>
-    <mergeCell ref="B96:B108"/>
-    <mergeCell ref="B109:B121"/>
-    <mergeCell ref="B122:B134"/>
-    <mergeCell ref="B135:B147"/>
-    <mergeCell ref="B148:B160"/>
-    <mergeCell ref="A57:A69"/>
-    <mergeCell ref="A70:A82"/>
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A3:A17"/>
-    <mergeCell ref="A18:A30"/>
-    <mergeCell ref="A31:A43"/>
-    <mergeCell ref="A44:A56"/>
-    <mergeCell ref="F3:F17"/>
-    <mergeCell ref="F18:F30"/>
-    <mergeCell ref="F31:F43"/>
-    <mergeCell ref="F44:F56"/>
   </mergeCells>
   <phoneticPr fontId="11" type="noConversion"/>
   <hyperlinks>

</xml_diff>